<commit_message>
Insurance 29/07/2019, Added Test Case
</commit_message>
<xml_diff>
--- a/Test Execution/Sangeetha/Testcase- Insurance.xlsx
+++ b/Test Execution/Sangeetha/Testcase- Insurance.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="734">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2541,6 +2541,136 @@
   </si>
   <si>
     <t>Select status "Approved"</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_104</t>
+  </si>
+  <si>
+    <t>Search OP Bills for 1st review</t>
+  </si>
+  <si>
+    <t>Precondition: OP Bill should be generated</t>
+  </si>
+  <si>
+    <t>Launch Application</t>
+  </si>
+  <si>
+    <t>Select Insurance module</t>
+  </si>
+  <si>
+    <t>Select 1st review tab</t>
+  </si>
+  <si>
+    <t>Select insurance and check OP Bills radio button and select search option</t>
+  </si>
+  <si>
+    <t>Insurance dashboard should be displayed</t>
+  </si>
+  <si>
+    <t>Search view with following fields to enter should be displayed:
+1) Billed from and to date
+2) Speciality
+3) Doctor
+4) TPA
+5) Insurance
+6) Type 
+7) Diagnosys Entry</t>
+  </si>
+  <si>
+    <t>Bill list based on selected fields should be displayed</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_105</t>
+  </si>
+  <si>
+    <t>Search IP Bills for 1st review</t>
+  </si>
+  <si>
+    <t>Precondition: IP Bill should be generated</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_106</t>
+  </si>
+  <si>
+    <t>Search Pharmacy Bills for 1st review</t>
+  </si>
+  <si>
+    <t>Precondition: Pharmacy Bill should be generated</t>
+  </si>
+  <si>
+    <t>Search OP Bills for Auditing</t>
+  </si>
+  <si>
+    <t>Search IP Bills for Auditing</t>
+  </si>
+  <si>
+    <t>Search Pharmacy Bills for Auditing</t>
+  </si>
+  <si>
+    <t>Patient id: NH00000595</t>
+  </si>
+  <si>
+    <t>Search IP Bills for 2nd review</t>
+  </si>
+  <si>
+    <t>Search OP Bills for 2nd review</t>
+  </si>
+  <si>
+    <t>Search Pharmacy Bills for 2nd review</t>
+  </si>
+  <si>
+    <t>Patient id: NH00000959</t>
+  </si>
+  <si>
+    <t>Patient id: NH00000123</t>
+  </si>
+  <si>
+    <t>Bill is not displaying</t>
+  </si>
+  <si>
+    <t>Select 2nd review tab</t>
+  </si>
+  <si>
+    <t>Select 2st review tab</t>
+  </si>
+  <si>
+    <t>Select Auditing tab</t>
+  </si>
+  <si>
+    <t>Precondition: Pharmacy Bill should be generated and passed 1nd and 2nd review</t>
+  </si>
+  <si>
+    <t>Precondition: IP Bill should be generated and passed 1st and 2nd Review</t>
+  </si>
+  <si>
+    <t>Precondition: OP Bill should be generated and passed 1st and 2nd review</t>
+  </si>
+  <si>
+    <t>Precondition: IP Bill should be generated and passed 1st review</t>
+  </si>
+  <si>
+    <t>Precondition: Pharmacy Bill should be generated and passed 1st  review</t>
+  </si>
+  <si>
+    <t>Precondition: OP Bill should be generated and passed 1st review</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_107</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_108</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_109</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_110</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_111</t>
+  </si>
+  <si>
+    <t>MED_Insurance_TC_112</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2737,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2635,6 +2765,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2667,7 +2803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2742,16 +2878,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3059,7 +3204,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3067,11 +3212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S780"/>
+  <dimension ref="A1:S834"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L673" sqref="L673"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3133,14 +3278,14 @@
       <c r="M1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="R1" s="29" t="s">
+      <c r="P1" s="30"/>
+      <c r="R1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="29"/>
+      <c r="S1" s="31"/>
     </row>
     <row r="2" spans="1:19" s="13" customFormat="1" ht="71.25" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -3171,14 +3316,14 @@
       </c>
       <c r="P2" s="4">
         <f>COUNTA(A:A)-1</f>
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="S2" s="6">
         <f>COUNTIF(L:L,"Pass")</f>
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="13" customFormat="1" ht="30">
@@ -3210,14 +3355,14 @@
       </c>
       <c r="P3" s="4">
         <f>COUNTA(L:L)-1</f>
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="S3" s="6">
         <f>COUNTIF(L:L,"Fail")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" ht="30">
@@ -3251,7 +3396,7 @@
       </c>
       <c r="S4" s="6">
         <f>COUNTIF(L:L,"Blocked")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="150">
@@ -3273,7 +3418,7 @@
       </c>
       <c r="S5" s="6">
         <f>COUNTA(M:M)-1</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="45">
@@ -5350,7 +5495,7 @@
         <v>337</v>
       </c>
       <c r="L165" s="4"/>
-      <c r="M165" s="30"/>
+      <c r="M165" s="28"/>
     </row>
     <row r="166" spans="1:13" ht="30">
       <c r="E166" s="11">
@@ -5368,7 +5513,7 @@
       <c r="L166" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M166" s="31" t="s">
+      <c r="M166" s="29" t="s">
         <v>404</v>
       </c>
     </row>
@@ -12581,9 +12726,687 @@
       </c>
     </row>
     <row r="780" spans="1:12">
-      <c r="J780" s="11"/>
-      <c r="K780" s="25"/>
+      <c r="A780" s="32"/>
+      <c r="B780" s="32"/>
+      <c r="C780" s="33"/>
+      <c r="D780" s="32"/>
+      <c r="E780" s="32"/>
+      <c r="F780" s="32"/>
+      <c r="G780" s="32"/>
+      <c r="H780" s="32"/>
+      <c r="I780" s="32"/>
+      <c r="J780" s="32"/>
+      <c r="K780" s="34"/>
       <c r="L780" s="22"/>
+    </row>
+    <row r="782" spans="1:12" ht="30">
+      <c r="A782" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="B782" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C782" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D782" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="F782" s="11" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="783" spans="1:12">
+      <c r="E783" s="11">
+        <v>1</v>
+      </c>
+      <c r="F783" s="11" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="784" spans="1:12" ht="30">
+      <c r="E784" s="11">
+        <v>2</v>
+      </c>
+      <c r="F784" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G784" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H784" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="785" spans="1:12" ht="150">
+      <c r="E785" s="11">
+        <v>3</v>
+      </c>
+      <c r="F785" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="G785" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H785" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="I785" s="11" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="786" spans="1:12" ht="30">
+      <c r="E786" s="11">
+        <v>4</v>
+      </c>
+      <c r="F786" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G786" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H786" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="K786" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L786" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="788" spans="1:12" ht="30">
+      <c r="A788" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="B788" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C788" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D788" s="11" t="s">
+        <v>704</v>
+      </c>
+      <c r="F788" s="11" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="789" spans="1:12">
+      <c r="E789" s="11">
+        <v>1</v>
+      </c>
+      <c r="F789" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H789" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="790" spans="1:12" ht="30">
+      <c r="E790" s="11">
+        <v>2</v>
+      </c>
+      <c r="F790" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G790" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H790" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="791" spans="1:12" ht="150">
+      <c r="E791" s="11">
+        <v>3</v>
+      </c>
+      <c r="F791" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="G791" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H791" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="I791" s="11" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="792" spans="1:12" ht="30">
+      <c r="E792" s="11">
+        <v>4</v>
+      </c>
+      <c r="F792" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G792" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H792" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="K792" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L792" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="794" spans="1:12" ht="30">
+      <c r="A794" s="11" t="s">
+        <v>706</v>
+      </c>
+      <c r="B794" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C794" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D794" s="11" t="s">
+        <v>707</v>
+      </c>
+      <c r="F794" s="11" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="795" spans="1:12">
+      <c r="E795" s="11">
+        <v>1</v>
+      </c>
+      <c r="F795" s="11" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="796" spans="1:12" ht="30">
+      <c r="E796" s="11">
+        <v>2</v>
+      </c>
+      <c r="F796" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G796" s="11" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="797" spans="1:12" ht="154.5" customHeight="1">
+      <c r="E797" s="11">
+        <v>3</v>
+      </c>
+      <c r="F797" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="G797" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="I797" s="11" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="798" spans="1:12" ht="30">
+      <c r="E798" s="11">
+        <v>4</v>
+      </c>
+      <c r="F798" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G798" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H798" s="11" t="s">
+        <v>718</v>
+      </c>
+      <c r="K798" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L798" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="800" spans="1:12" ht="30">
+      <c r="A800" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="B800" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C800" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D800" s="11" t="s">
+        <v>714</v>
+      </c>
+      <c r="F800" s="11" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="801" spans="1:13">
+      <c r="E801" s="11">
+        <v>1</v>
+      </c>
+      <c r="F801" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H801" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="802" spans="1:13" ht="30">
+      <c r="E802" s="11">
+        <v>2</v>
+      </c>
+      <c r="F802" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G802" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H802" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="803" spans="1:13" ht="155.25" customHeight="1">
+      <c r="E803" s="11">
+        <v>3</v>
+      </c>
+      <c r="F803" s="11" t="s">
+        <v>719</v>
+      </c>
+      <c r="G803" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H803" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="804" spans="1:13" ht="30">
+      <c r="E804" s="11">
+        <v>4</v>
+      </c>
+      <c r="F804" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G804" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H804" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="L804" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="M804" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="806" spans="1:13" ht="30">
+      <c r="A806" s="11" t="s">
+        <v>729</v>
+      </c>
+      <c r="B806" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C806" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D806" s="11" t="s">
+        <v>713</v>
+      </c>
+      <c r="F806" s="11" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="807" spans="1:13">
+      <c r="E807" s="11">
+        <v>1</v>
+      </c>
+      <c r="F807" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H807" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="808" spans="1:13" ht="30">
+      <c r="E808" s="11">
+        <v>2</v>
+      </c>
+      <c r="F808" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G808" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H808" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="809" spans="1:13" ht="157.5" customHeight="1">
+      <c r="E809" s="11">
+        <v>3</v>
+      </c>
+      <c r="F809" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="G809" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H809" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="I809" s="11" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="810" spans="1:13" ht="30">
+      <c r="E810" s="11">
+        <v>4</v>
+      </c>
+      <c r="F810" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G810" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H810" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="K810" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L810" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="812" spans="1:13" ht="30">
+      <c r="A812" s="11" t="s">
+        <v>730</v>
+      </c>
+      <c r="B812" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C812" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D812" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="F812" s="11" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="813" spans="1:13">
+      <c r="E813" s="11">
+        <v>1</v>
+      </c>
+      <c r="F813" s="11" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="814" spans="1:13" ht="30">
+      <c r="E814" s="11">
+        <v>2</v>
+      </c>
+      <c r="F814" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G814" s="11" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="815" spans="1:13" ht="150">
+      <c r="E815" s="11">
+        <v>3</v>
+      </c>
+      <c r="F815" s="11" t="s">
+        <v>719</v>
+      </c>
+      <c r="G815" s="11" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="816" spans="1:13" ht="30">
+      <c r="E816" s="11">
+        <v>4</v>
+      </c>
+      <c r="F816" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G816" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="K816" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L816" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="818" spans="1:12" ht="45">
+      <c r="A818" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="B818" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C818" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D818" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="F818" s="11" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="819" spans="1:12">
+      <c r="E819" s="11">
+        <v>1</v>
+      </c>
+      <c r="F819" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H819" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="820" spans="1:12" ht="30">
+      <c r="E820" s="11">
+        <v>2</v>
+      </c>
+      <c r="F820" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G820" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H820" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="821" spans="1:12" ht="150">
+      <c r="E821" s="11">
+        <v>3</v>
+      </c>
+      <c r="F821" s="11" t="s">
+        <v>721</v>
+      </c>
+      <c r="G821" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H821" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="822" spans="1:12" ht="30">
+      <c r="E822" s="11">
+        <v>4</v>
+      </c>
+      <c r="F822" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G822" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H822" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="K822" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L822" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="824" spans="1:12" ht="45">
+      <c r="A824" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="B824" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C824" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D824" s="11" t="s">
+        <v>710</v>
+      </c>
+      <c r="F824" s="11" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="825" spans="1:12">
+      <c r="E825" s="11">
+        <v>1</v>
+      </c>
+      <c r="F825" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H825" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="826" spans="1:12" ht="30">
+      <c r="E826" s="11">
+        <v>2</v>
+      </c>
+      <c r="F826" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G826" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H826" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="827" spans="1:12" ht="150">
+      <c r="E827" s="11">
+        <v>3</v>
+      </c>
+      <c r="F827" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="G827" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H827" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="828" spans="1:12" ht="30">
+      <c r="E828" s="11">
+        <v>4</v>
+      </c>
+      <c r="F828" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G828" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="H828" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="K828" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L828" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="830" spans="1:12" ht="45">
+      <c r="A830" s="11" t="s">
+        <v>733</v>
+      </c>
+      <c r="B830" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C830" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D830" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="F830" s="11" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="831" spans="1:12">
+      <c r="E831" s="11">
+        <v>1</v>
+      </c>
+      <c r="F831" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="H831" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="832" spans="1:12" ht="30">
+      <c r="E832" s="11">
+        <v>2</v>
+      </c>
+      <c r="F832" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G832" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="H832" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="833" spans="5:12" ht="150">
+      <c r="E833" s="11">
+        <v>3</v>
+      </c>
+      <c r="F833" s="11" t="s">
+        <v>721</v>
+      </c>
+      <c r="G833" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="H833" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="834" spans="5:12" ht="30">
+      <c r="E834" s="11">
+        <v>4</v>
+      </c>
+      <c r="F834" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="G834" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="K834" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="L834" s="22" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="L1:L780"/>
@@ -12593,10 +13416,16 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K781:K1048576 K56:K398 C58:C110 C113:C333 C2:C47 C49:C56 K2:K47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L822 L834 L828 L816 L810 L399:L622 L624:L722 L724:L780 L2:L47 L56:L397 L786 L792 M804 L798">
+      <formula1>"Pass, Fail, Blocked"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K822 K834 K828 K816 K810 K691 K779 K773 K732 K742 K750 K758 K766 K786 K792 L804 K798">
+      <formula1>"Anjana S, Salini S, Preethi Pathrose, Leona, Parvathy, Raziya, Rijo"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K47 K823 K817:K821 K829:K833 K825:K827 K835:K1048576 K811:K815 K799:K809 C58:C110 C113:C333 C2:C47 C49:C56 K781:K785 K787:K791 K793:K797 K56:K398">
       <formula1>"Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C776:C779 C769:C772 C761:C764 C753:C756 C745:C748 C737:C740 K538 K526 K520 K399:K515 C670:C674 C399:C667 C718:C727 C712:C716 C706:C710 C700:C704 C694:C698 C688:C692 C682:C686 C676:C680 C732:C735">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C776:C779 C769:C772 C761:C764 C753:C756 C745:C748 C737:C740 K538 K526 K520 K399:K515 C670:C674 C399:C667 C718:C727 C712:C716 C706:C710 C700:C704 C694:C698 C688:C692 C682:C686 C676:C680 C732:C735 C782 C788 C794 C800 C806 C812 C818 C824 C830 C836">
       <formula1>"Anjana S, Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C780 C773:C774 C765:C767 C757:C759 C749:C751 C741:C743 C668:C669 C717 C711 C705 C699 C693 C687 C681 C675 C728:C731 C736">
@@ -12604,12 +13433,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B399 B405:B406 B412:B413 B420 B14:B16 B8 B22:B25 B30:B32 B38:B40 B135 B127 B119 B125 B113 B103:B104 B97 B95 B89 B87 B80:B81 B149 B143 B214:B215 B196 B182 B169 B167 B72:B74 B66 B209 B203 B58 B56 B49 B189 B177 B160 B157 B151 B133 B141 B221 B237:B238 B228:B230 B240 B254:B255 B247 B263 B311 B319:B320 B287 B326:B327 B289 B295:B296 B281 B302:B303 B309 B273 B279 B2">
       <formula1>"CAS/ Appointment, Out Patient, Care Desk, EMR, Lab &amp; General Billing, Pharmacy Billing, Lab Results, Radiology, Insurance Desk, Casualty, MRD, In Patient, Nursing Station, Theatre, Indent, Store Management"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L399:L622 L624:L722 L724:L780 L2:L47 L56:L397">
-      <formula1>"Pass, Fail, Blocked"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K691 K779 K773 K732 K742 K750 K758 K766">
-      <formula1>"Anjana S, Salini S, Preethi Pathrose, Leona, Parvathy, Raziya, Rijo"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K516:K519 K780 K774:K778 K767:K772 K539:K690 K521:K525 K724 K719 K712 K706 K700 K527:K537 K733:K741 K743:K749 K751:K757 K759:K765 K692:K695">
       <formula1>"Anjana S, Salini S, Preethi J, Leona, Parvathy, Raziya, Rijo"</formula1>

</xml_diff>